<commit_message>
rajout des fonctions sur les articles
</commit_message>
<xml_diff>
--- a/RESSOURCES/DB_ARTICLES.xlsx
+++ b/RESSOURCES/DB_ARTICLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3175C411-6C96-481F-B91A-1FF4B804039D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A7A67-46A2-4BFA-A31F-44E61B23E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6394,7 +6394,7 @@
   <dimension ref="A1:F870"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add unit and category ID retrieval in article import and enable Flask auto-reload
</commit_message>
<xml_diff>
--- a/RESSOURCES/DB_ARTICLES.xlsx
+++ b/RESSOURCES/DB_ARTICLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A7A67-46A2-4BFA-A31F-44E61B23E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C065EFD-4F22-475C-9707-428CEF1C5CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27285" yWindow="1515" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6394,7 +6394,7 @@
   <dimension ref="A1:F870"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add new Excel file for product packaging details by brand
</commit_message>
<xml_diff>
--- a/RESSOURCES/DB_ARTICLES.xlsx
+++ b/RESSOURCES/DB_ARTICLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C065EFD-4F22-475C-9707-428CEF1C5CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DC0CA8-8EF4-4CC4-AF84-3503EC3E4016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27285" yWindow="1515" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$870</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="2005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3741" uniqueCount="2007">
   <si>
     <t>code</t>
   </si>
@@ -6046,6 +6046,12 @@
   </si>
   <si>
     <t>PIECE</t>
+  </si>
+  <si>
+    <t>MARQUE</t>
+  </si>
+  <si>
+    <t>Biochamps RHF</t>
   </si>
 </sst>
 </file>
@@ -6391,10 +6397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F870"/>
+  <dimension ref="A1:G870"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6407,7 +6413,7 @@
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6426,8 +6432,11 @@
       <c r="F1" s="1" t="s">
         <v>2000</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1136</v>
       </c>
@@ -6445,7 +6454,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1137</v>
       </c>
@@ -6463,7 +6472,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1138</v>
       </c>
@@ -6481,7 +6490,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1139</v>
       </c>
@@ -6499,7 +6508,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1140</v>
       </c>
@@ -6519,7 +6528,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1141</v>
       </c>
@@ -6539,7 +6548,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1142</v>
       </c>
@@ -6559,7 +6568,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1143</v>
       </c>
@@ -6577,7 +6586,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1144</v>
       </c>
@@ -6595,7 +6604,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1145</v>
       </c>
@@ -6613,7 +6622,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1146</v>
       </c>
@@ -6631,7 +6640,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1147</v>
       </c>
@@ -6649,7 +6658,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1148</v>
       </c>
@@ -6667,7 +6676,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1149</v>
       </c>
@@ -6685,7 +6694,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1150</v>
       </c>
@@ -21176,7 +21185,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="801" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A801" s="3" t="s">
         <v>1930</v>
       </c>
@@ -21196,7 +21205,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="802" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A802" s="3" t="s">
         <v>1931</v>
       </c>
@@ -21216,7 +21225,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="803" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A803" s="3" t="s">
         <v>1932</v>
       </c>
@@ -21236,7 +21245,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="804" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A804" s="3" t="s">
         <v>1933</v>
       </c>
@@ -21256,7 +21265,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="805" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A805" s="3" t="s">
         <v>1934</v>
       </c>
@@ -21276,7 +21285,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="806" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A806" s="3" t="s">
         <v>1935</v>
       </c>
@@ -21296,7 +21305,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="807" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A807" s="3" t="s">
         <v>1936</v>
       </c>
@@ -21316,7 +21325,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="808" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A808" s="3" t="s">
         <v>1937</v>
       </c>
@@ -21336,7 +21345,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="809" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A809" s="3" t="s">
         <v>1938</v>
       </c>
@@ -21356,7 +21365,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="810" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A810" s="3" t="s">
         <v>1939</v>
       </c>
@@ -21376,7 +21385,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="811" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A811" s="3" t="s">
         <v>1940</v>
       </c>
@@ -21396,7 +21405,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="812" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A812" s="3" t="s">
         <v>1941</v>
       </c>
@@ -21416,7 +21425,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="813" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A813" s="3" t="s">
         <v>1942</v>
       </c>
@@ -21436,7 +21445,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="814" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A814" s="3" t="s">
         <v>1943</v>
       </c>
@@ -21456,7 +21465,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="815" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A815" s="3" t="s">
         <v>1944</v>
       </c>
@@ -21476,7 +21485,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="816" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A816" s="3" t="s">
         <v>1945</v>
       </c>
@@ -21495,8 +21504,11 @@
       <c r="F816" s="2" t="s">
         <v>2002</v>
       </c>
-    </row>
-    <row r="817" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G816" s="2" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="817" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A817" s="3" t="s">
         <v>1946</v>
       </c>
@@ -21515,8 +21527,11 @@
       <c r="F817" s="2" t="s">
         <v>2002</v>
       </c>
-    </row>
-    <row r="818" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G817" s="2" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="818" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A818" s="3" t="s">
         <v>1947</v>
       </c>
@@ -21536,7 +21551,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="819" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A819" s="3" t="s">
         <v>1948</v>
       </c>
@@ -21556,7 +21571,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="820" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A820" s="3" t="s">
         <v>1949</v>
       </c>
@@ -21576,7 +21591,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="821" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A821" s="3" t="s">
         <v>1950</v>
       </c>
@@ -21596,7 +21611,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="822" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A822" s="3" t="s">
         <v>1951</v>
       </c>
@@ -21615,8 +21630,11 @@
       <c r="F822" s="2" t="s">
         <v>2002</v>
       </c>
-    </row>
-    <row r="823" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G822" s="2" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="823" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A823" s="3" t="s">
         <v>1952</v>
       </c>
@@ -21636,7 +21654,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="824" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A824" s="3" t="s">
         <v>1953</v>
       </c>
@@ -21656,7 +21674,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="825" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A825" s="3" t="s">
         <v>1954</v>
       </c>
@@ -21676,7 +21694,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="826" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A826" s="3" t="s">
         <v>1955</v>
       </c>
@@ -21696,7 +21714,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="827" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="827" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A827" s="3" t="s">
         <v>1956</v>
       </c>
@@ -21716,7 +21734,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="828" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A828" s="3" t="s">
         <v>1957</v>
       </c>
@@ -21736,7 +21754,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="829" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="829" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A829" s="3" t="s">
         <v>1958</v>
       </c>
@@ -21756,7 +21774,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="830" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A830" s="3" t="s">
         <v>1959</v>
       </c>
@@ -21776,7 +21794,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="831" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A831" s="3" t="s">
         <v>1960</v>
       </c>
@@ -21796,7 +21814,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="832" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A832" s="3" t="s">
         <v>1961</v>
       </c>

</xml_diff>